<commit_message>
Testes possitivo e negativo com os asserts no cenario de Pesquisa com a lupa
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/appium/testData/TestData.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/appium/testData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caique.oliveira\eclipse-workspace\AppiumTDD\src\main\java\br\com\rsinet\hub_tdd\appium\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89908150-6BB9-4C27-9A62-6F0C42DD4B7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DD57EC-5744-445A-816D-28FECE786876}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="2340" windowWidth="16110" windowHeight="7875" activeTab="1" xr2:uid="{A9FA70BE-A689-4F6B-9AF8-812824F582B6}"/>
+    <workbookView xWindow="-19695" yWindow="915" windowWidth="16110" windowHeight="7875" xr2:uid="{A9FA70BE-A689-4F6B-9AF8-812824F582B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ECC51B8-0D12-4ED7-B203-D3656A8C93F0}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -609,13 +609,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141451B3-9CBA-429A-9675-639952A6C031}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>